<commit_message>
Improved handing of dc init to preserve existing metadata
</commit_message>
<xml_diff>
--- a/deployable examples/reusable_settings_only/src/reusable_settings_only.xlsx
+++ b/deployable examples/reusable_settings_only/src/reusable_settings_only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshbregman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbreg\OneDrive\Documents\GitHub\mdatp-devicecontrol\deployable examples\reusable_settings_only\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B895C2A1-F93C-4E85-8479-305EE121FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70228F0-C2E0-454D-8C82-13806DD0D80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16380" windowHeight="10260" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
   </bookViews>
   <sheets>
     <sheet name="Authorized USBs" sheetId="18" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>046d_0825</t>
   </si>
   <si>
-    <t>05ac_12a0</t>
-  </si>
-  <si>
     <t>Device A</t>
   </si>
   <si>
@@ -94,6 +91,15 @@
   </si>
   <si>
     <t>Descriptor Value Name</t>
+  </si>
+  <si>
+    <t>AAAA_BBBB</t>
+  </si>
+  <si>
+    <t>Device F</t>
+  </si>
+  <si>
+    <t>FFFF_2222</t>
   </si>
 </sst>
 </file>
@@ -103,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,77 +534,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5CE340-DBC1-4308-9AB7-93733A7E1F01}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.76953125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21.1328125" customWidth="1"/>
+    <col min="2" max="2" width="25.75" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4">
       <c r="A10" s="4"/>
       <c r="B10" s="7"/>
     </row>
@@ -616,12 +628,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.953125" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -643,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
     </row>
   </sheetData>
@@ -657,7 +669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -669,7 +681,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -683,7 +695,7 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>